<commit_message>
added all new training materials; updated readme accordingly
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/plotting_settings.xlsx
+++ b/2_REVUB_control_files/plotting_settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/23006 REVUB tutorial/Training dataset/sheets to be provided/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{BE585F5E-6B91-4E61-AA71-0D4160623741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12F76584-D0B9-4F0F-8E98-9DBC8CF8344D}"/>
+  <xr:revisionPtr revIDLastSave="249" documentId="8_{BE585F5E-6B91-4E61-AA71-0D4160623741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B65449A1-33CF-4E96-91B3-BABA07342C63}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2DE6606B-B2DA-40D4-9284-557EFCF05F90}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>plot_HPP</t>
   </si>
@@ -61,9 +61,6 @@
     <t>chosen_load</t>
   </si>
   <si>
-    <t>Bui</t>
-  </si>
-  <si>
     <t>for hourly graph: choose month to plot (1 = Jan; 2 = Feb; etc.)</t>
   </si>
   <si>
@@ -100,7 +97,13 @@
     <t>P_total_av</t>
   </si>
   <si>
-    <t>Buyo</t>
+    <t>enter here the name of the target load curve to be used for the plot here</t>
+  </si>
+  <si>
+    <t>[name 1]</t>
+  </si>
+  <si>
+    <t>[name 2]</t>
   </si>
   <si>
     <r>
@@ -119,15 +122,6 @@
     </r>
   </si>
   <si>
-    <t>enter the names of the hydropower plants to include in this plot in row 2, starting in column B</t>
-  </si>
-  <si>
-    <t>enter here the name of the target load curve to be used for the plot here</t>
-  </si>
-  <si>
-    <t>in the below rows, enter single values in column B</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">in this row, enter all months (using numbers 1-12, one per cell) for which to plot release rules </t>
     </r>
@@ -143,6 +137,12 @@
   </si>
   <si>
     <t>in this row, enter all hours of the day (using numbers 0-23, one per cell) for which to plot release rules →</t>
+  </si>
+  <si>
+    <t>enter the names of the hydropower plants to include in this plot in row 2, starting in column B</t>
+  </si>
+  <si>
+    <t>in the below rows, enter single values in column B</t>
   </si>
 </sst>
 </file>
@@ -167,13 +167,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -184,6 +177,13 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -245,17 +245,17 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -273,6 +273,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -575,111 +579,95 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>15</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>4</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>3</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCC4198-7EC1-402D-B6B2-C37644E56842}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +680,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,100 +690,88 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3">
-        <v>400</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved and completed cascade calculation, now allowing coupled simulation of up- and downstream plants of flexibility-providing HPPs. (Note: manual and training dataset not yet updated to this latest development.)
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/plotting_settings.xlsx
+++ b/2_REVUB_control_files/plotting_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/24006 Ecuador crisis energética/Investigación/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="8_{BE585F5E-6B91-4E61-AA71-0D4160623741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{644498A7-F105-4704-AFA4-30DB99F1D40D}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{D184A4C5-B06D-4DCB-A49D-05833EDCF5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B333C57F-AEBD-4561-9431-F06048FAB4CE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2DE6606B-B2DA-40D4-9284-557EFCF05F90}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>plot_HPP</t>
   </si>
@@ -97,15 +97,6 @@
     <t>P_total_av</t>
   </si>
   <si>
-    <t>enter here the name of the target load curve to be used for the plot here</t>
-  </si>
-  <si>
-    <t>[name 1]</t>
-  </si>
-  <si>
-    <t>[name 2]</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">for hourly graph: number of days to show, starting at </t>
     </r>
@@ -145,31 +136,49 @@
     <t>in the below rows, enter single values in column B</t>
   </si>
   <si>
+    <t>plot_RoR_part</t>
+  </si>
+  <si>
     <t>set to 1 to plot run-of-river component of electricity generation, or to 0 to leave out this component</t>
   </si>
   <si>
-    <t>plot_RoR_part</t>
-  </si>
-  <si>
     <t>Figure1_on</t>
   </si>
   <si>
+    <t>Figure2_on</t>
+  </si>
+  <si>
+    <t>Figure3_on</t>
+  </si>
+  <si>
+    <t>Figure4_on</t>
+  </si>
+  <si>
+    <t>Figure5_on</t>
+  </si>
+  <si>
+    <t>Figure6_on</t>
+  </si>
+  <si>
+    <t>Figure7_on</t>
+  </si>
+  <si>
+    <t>Figure8_on</t>
+  </si>
+  <si>
+    <t>Figure9_on</t>
+  </si>
+  <si>
     <t>set to 1 to plot bathymetry relations, or to 0 to turn off</t>
   </si>
   <si>
-    <t>Figure2_on</t>
-  </si>
-  <si>
     <t>set to 1 to plot hydraulic head and inflow/outflow IQ ranges, or to 0 to turn off</t>
   </si>
   <si>
-    <t>Figure3_on</t>
-  </si>
-  <si>
     <t>set to 1 to plot full time series of reservoir volume and inflow/outflow, or to 0 to turn off</t>
   </si>
   <si>
-    <t>Figure4_on</t>
+    <t>set to 1 to plot year-by-year power generation, or to 0 to turn off</t>
   </si>
   <si>
     <r>
@@ -198,15 +207,6 @@
     </r>
   </si>
   <si>
-    <t>Figure5_on</t>
-  </si>
-  <si>
-    <t>set to 1 to plot year-by-year power generation, or to 0 to turn off</t>
-  </si>
-  <si>
-    <t>Figure6_on</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">set to 1 to plot hourly power generation from date </t>
     </r>
@@ -254,7 +254,48 @@
     </r>
   </si>
   <si>
-    <t>Figure7_on</t>
+    <t>set to 1 to plot hydroturbine use statistics, or to 0 to turn off</t>
+  </si>
+  <si>
+    <r>
+      <t>set to 1 to plot operational regime statistics, or to 0 to turn off [</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: currently only available for BAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>set to 1 to include a bold black line for ELCC, or to 0 to leave out</t>
+  </si>
+  <si>
+    <t>plot_ELCC_line</t>
+  </si>
+  <si>
+    <t>Ecuador normalised</t>
+  </si>
+  <si>
+    <t>Mazar upstream s+w overpr</t>
+  </si>
+  <si>
+    <t>Paute-Molino cascade s+w flow_corr overpr</t>
   </si>
   <si>
     <r>
@@ -279,21 +320,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, or to 0 to turn off</t>
-    </r>
-  </si>
-  <si>
-    <t>Figure8_on</t>
-  </si>
-  <si>
-    <t>set to 1 to plot hydroturbine use statistics, or to 0 to turn off</t>
-  </si>
-  <si>
-    <t>Figure9_on</t>
-  </si>
-  <si>
-    <r>
-      <t>set to 1 to plot operational regime statistics, or to 0 to turn off [</t>
+      <t xml:space="preserve">, or to 0 to turn off </t>
     </r>
     <r>
       <rPr>
@@ -304,25 +331,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note: currently only available for BAL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
+      <t>[Note: currently only available for BAL]</t>
+    </r>
+  </si>
+  <si>
+    <t>Sopladora downstream</t>
+  </si>
+  <si>
+    <t>plot_ELCC_line_multiple</t>
+  </si>
+  <si>
+    <t>enter here the name of the target load curve to be used for the plot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +380,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,12 +450,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -429,8 +464,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -749,23 +789,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D042E9-2187-43E7-85C1-E373CF44E8EE}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="C1" t="s">
         <v>10</v>
       </c>
@@ -774,7 +816,9 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>12</v>
+      </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -783,7 +827,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>11</v>
+      </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
@@ -792,7 +838,9 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>12</v>
+      </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -801,99 +849,132 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -904,10 +985,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCC4198-7EC1-402D-B6B2-C37644E56842}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,20 +998,29 @@
     <col min="3" max="3" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -940,33 +1030,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B677A325-0757-43AE-BF2B-DF4DC9D55A1C}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3"/>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -980,14 +1074,16 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>12</v>
+      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -996,7 +1092,9 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>11</v>
+      </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -1005,7 +1103,9 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>12</v>
+      </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -1014,27 +1114,44 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>3000</v>
+      </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first commit version 1.1.0 including cascade calculation logic
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/plotting_settings.xlsx
+++ b/2_REVUB_control_files/plotting_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/24006 Ecuador crisis energética/Investigación/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{D184A4C5-B06D-4DCB-A49D-05833EDCF5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B333C57F-AEBD-4561-9431-F06048FAB4CE}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="13_ncr:1_{D184A4C5-B06D-4DCB-A49D-05833EDCF5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F83D8F3A-27EF-44BC-A171-1DC16B228EDC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2DE6606B-B2DA-40D4-9284-557EFCF05F90}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>plot_HPP</t>
   </si>
@@ -289,15 +289,6 @@
     <t>plot_ELCC_line</t>
   </si>
   <si>
-    <t>Ecuador normalised</t>
-  </si>
-  <si>
-    <t>Mazar upstream s+w overpr</t>
-  </si>
-  <si>
-    <t>Paute-Molino cascade s+w flow_corr overpr</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">set to 1 to plot regulated reservoir release statistics [see worksheet </t>
     </r>
@@ -335,13 +326,19 @@
     </r>
   </si>
   <si>
-    <t>Sopladora downstream</t>
-  </si>
-  <si>
     <t>plot_ELCC_line_multiple</t>
   </si>
   <si>
     <t>enter here the name of the target load curve to be used for the plot</t>
+  </si>
+  <si>
+    <t>[name 1]</t>
+  </si>
+  <si>
+    <t>[name 2]</t>
+  </si>
+  <si>
+    <t>[name 3]</t>
   </si>
 </sst>
 </file>
@@ -486,10 +483,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -792,7 +785,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -806,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
@@ -816,9 +809,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>12</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -827,9 +818,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>11</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" t="s">
         <v>7</v>
       </c>
@@ -838,9 +827,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>12</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -849,9 +836,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>19</v>
       </c>
@@ -860,9 +845,7 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
+      <c r="B6" s="6"/>
       <c r="C6" t="s">
         <v>25</v>
       </c>
@@ -871,9 +854,7 @@
       <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
+      <c r="B7" s="6"/>
       <c r="C7" t="s">
         <v>43</v>
       </c>
@@ -882,9 +863,7 @@
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
+      <c r="B8" s="6"/>
       <c r="C8" t="s">
         <v>35</v>
       </c>
@@ -893,9 +872,7 @@
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="6">
-        <v>0</v>
-      </c>
+      <c r="B9" s="6"/>
       <c r="C9" t="s">
         <v>36</v>
       </c>
@@ -904,9 +881,7 @@
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
+      <c r="B10" s="6"/>
       <c r="C10" t="s">
         <v>37</v>
       </c>
@@ -915,9 +890,7 @@
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
+      <c r="B11" s="6"/>
       <c r="C11" t="s">
         <v>39</v>
       </c>
@@ -926,9 +899,7 @@
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
+      <c r="B12" s="6"/>
       <c r="C12" t="s">
         <v>38</v>
       </c>
@@ -937,9 +908,7 @@
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
+      <c r="B13" s="6"/>
       <c r="C13" t="s">
         <v>40</v>
       </c>
@@ -948,20 +917,16 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
+      <c r="B14" s="6"/>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
+      <c r="B15" s="6"/>
       <c r="C15" t="s">
         <v>41</v>
       </c>
@@ -970,9 +935,7 @@
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
+      <c r="B16" s="6"/>
       <c r="C16" t="s">
         <v>42</v>
       </c>
@@ -985,10 +948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCC4198-7EC1-402D-B6B2-C37644E56842}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -998,29 +961,20 @@
     <col min="3" max="3" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1033,7 +987,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1048,18 +1002,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1081,9 +1035,7 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
-        <v>12</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -1092,9 +1044,7 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2">
-        <v>11</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -1103,9 +1053,7 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2">
-        <v>12</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -1114,9 +1062,7 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>19</v>
       </c>
@@ -1125,31 +1071,25 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2">
-        <v>3000</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B10" s="6"/>
       <c r="C10" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
allowing dynamic demand and capacity time series in plotting full power mix sheet; addition of ramping envelopes (update of manual to follow)
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/plotting_settings.xlsx
+++ b/2_REVUB_control_files/plotting_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="13_ncr:1_{D184A4C5-B06D-4DCB-A49D-05833EDCF5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F83D8F3A-27EF-44BC-A171-1DC16B228EDC}"/>
+  <xr:revisionPtr revIDLastSave="491" documentId="13_ncr:1_{D184A4C5-B06D-4DCB-A49D-05833EDCF5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F789E43-774C-466F-B2AD-6B54CDB5A0C6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2DE6606B-B2DA-40D4-9284-557EFCF05F90}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>plot_HPP</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>exact name of hydropower plant to plot</t>
-  </si>
-  <si>
-    <t>total average load (MW) assumed for graph of full power mix (all non-hydro + VRE is assumed thermal power)</t>
   </si>
   <si>
     <t>plot_rules_hr</t>
@@ -133,9 +130,6 @@
     <t>enter the names of the hydropower plants to include in this plot in row 2, starting in column B</t>
   </si>
   <si>
-    <t>in the below rows, enter single values in column B</t>
-  </si>
-  <si>
     <t>plot_RoR_part</t>
   </si>
   <si>
@@ -332,20 +326,62 @@
     <t>enter here the name of the target load curve to be used for the plot</t>
   </si>
   <si>
-    <t>[name 1]</t>
-  </si>
-  <si>
-    <t>[name 2]</t>
-  </si>
-  <si>
-    <t>[name 3]</t>
+    <t>number of hours to include in ramping envelopes</t>
+  </si>
+  <si>
+    <t>P_r_total_thermal</t>
+  </si>
+  <si>
+    <t>total average load (MW) assumed for graph of full power mix</t>
+  </si>
+  <si>
+    <t>P_total_av_series</t>
+  </si>
+  <si>
+    <t>[year 1]</t>
+  </si>
+  <si>
+    <t>[year 2]</t>
+  </si>
+  <si>
+    <t>&amp;c…</t>
+  </si>
+  <si>
+    <t>[plotting] set visualisation parameters</t>
+  </si>
+  <si>
+    <t>choose_demand_type</t>
+  </si>
+  <si>
+    <t>P_r_total_thermal_series</t>
+  </si>
+  <si>
+    <t>[static: demand]</t>
+  </si>
+  <si>
+    <t>[static: non-hydro capacity]</t>
+  </si>
+  <si>
+    <t>[dynamic: demand] enter a time series of average demand (MW) for each year in the simulation</t>
+  </si>
+  <si>
+    <t>[dynamic: non-hydro capacity] enter a time series of available capacity (MW) of flexible non-hydro assets (thermal, imports, &amp;c.)</t>
+  </si>
+  <si>
+    <t>total flexible non-hydro (thermal, importc, &amp;c.) capacity assumed available (MW)</t>
+  </si>
+  <si>
+    <t>[choose] whether to use static (=0; same year-to-year) or dynamic (=1; time series) demand and capacity</t>
+  </si>
+  <si>
+    <t>plot_ramping_range</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +421,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -453,7 +496,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -465,6 +508,13 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
@@ -483,6 +533,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -785,7 +839,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,9 +852,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="B1" s="5"/>
       <c r="C1" t="s">
         <v>10</v>
       </c>
@@ -838,106 +890,106 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +1003,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -966,15 +1018,15 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -984,114 +1036,227 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B677A325-0757-43AE-BF2B-DF4DC9D55A1C}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
     <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" t="s">
-        <v>43</v>
+      <c r="B27" s="5"/>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>